<commit_message>
BGM can change during dialogue.
Author: James Iwamasa.

-Some more improvements on audio framework. Designers can now specify what
bgm should play for each line of dialogue ("_" specifies no change).
-Todo: Spell sfx, UI sfx, and Battle sfx.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/gameflow.xlsx
+++ b/Typocrypha/Assets/excel/gameflow.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>INTRO</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>MUSIC</t>
+  </si>
+  <si>
+    <t>frogs</t>
+  </si>
+  <si>
+    <t>_</t>
   </si>
 </sst>
 </file>
@@ -450,20 +456,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -471,12 +477,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -487,155 +493,182 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -643,47 +676,22 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Starting implementation of mid-battle cutscenes.
-Currently, cutscenes can be triggered when an enemy's (or the player's)
health goes below a certain percentage. The Battle scene can recognize
these events, but does not yet play the Cutscene.
-This information is stored in the gameflow file.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/gameflow.xlsx
+++ b/Typocrypha/Assets/excel/gameflow.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
   <si>
     <t>INTRO</t>
   </si>
@@ -68,43 +68,88 @@
     <t>frog_mario</t>
   </si>
   <si>
+    <t>Hey you! You're walking in the wrong part of town.</t>
+  </si>
+  <si>
+    <t>Ribbit Ribbit! (Yeah frog-face! Wrong part of town!)</t>
+  </si>
+  <si>
+    <t>Let's get em!</t>
+  </si>
+  <si>
+    <t>(He's not moving)</t>
+  </si>
+  <si>
+    <t>jazzy_retro_battle_theme</t>
+  </si>
+  <si>
+    <t>sample_incomplete_war_remix</t>
+  </si>
+  <si>
+    <t>second_hand</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>frogs</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>MIDDLE_HEALTH</t>
+  </si>
+  <si>
+    <t>RIGHT_HEALTH</t>
+  </si>
+  <si>
+    <t>PLAYER_HEALTH</t>
+  </si>
+  <si>
+    <t>INTERRUPT</t>
+  </si>
+  <si>
+    <t>END_INTERRUPT</t>
+  </si>
+  <si>
+    <t>Ha! Feel the wrath of Tanuki and Frog!</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Did you just kill the Evil Eye? Did- Did you win?</t>
+  </si>
+  <si>
+    <t>INTERRUPT_END</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Holy crap.</t>
+  </si>
+  <si>
+    <t>Ribbit! (Wow, you're actually killing the Evil Eye!)</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>Ugh! How are you so powerful? You even killed Frog!</t>
+  </si>
+  <si>
+    <t>Ah! You have defeated me!</t>
+  </si>
+  <si>
+    <t>Bleh. (ded)</t>
+  </si>
+  <si>
+    <t>Ribbit Ribbit Rrrrrrribbit! (Frog is actually just making frog sounds right now)</t>
+  </si>
+  <si>
     <t>Slime</t>
-  </si>
-  <si>
-    <t>Hey you! You're walking in the wrong part of town.</t>
-  </si>
-  <si>
-    <t>Ribbit Ribbit! (Yeah frog-face! Wrong part of town!)</t>
-  </si>
-  <si>
-    <t>Let's get em!</t>
-  </si>
-  <si>
-    <t>I'm out of here!</t>
-  </si>
-  <si>
-    <t>(He's not moving)</t>
-  </si>
-  <si>
-    <t>Oh my god. You killed Frog!</t>
-  </si>
-  <si>
-    <t>jazzy_retro_battle_theme</t>
-  </si>
-  <si>
-    <t>sample_incomplete_war_remix</t>
-  </si>
-  <si>
-    <t>second_hand</t>
-  </si>
-  <si>
-    <t>MUSIC</t>
-  </si>
-  <si>
-    <t>frogs</t>
-  </si>
-  <si>
-    <t>_</t>
   </si>
 </sst>
 </file>
@@ -456,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -517,13 +562,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -534,13 +579,13 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -551,13 +596,13 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -575,10 +620,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,7 +631,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -607,31 +652,52 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -642,7 +708,7 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -656,42 +722,199 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>0.75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved Allies, Added Ally Casting, Added Allies to bigger system
-Added AllyDatabase.cs (similar to EnemyDatabase.cs) with appropriate excel (and.txt) and building code
-Added AllyDatabase (and ALLY flag) to loadgameflow.cs, specifically in parseBattle()
-Correctly built ally objects (using prefabs) in battlemanager.cs
-Correctly handled Ally spellcasting in battlemanager.cs (edited playerCast and NPC_cast)
-Correctly handled Ally casts in spelldictionary (add friend/* spell typing)
-Correctly handled ally spells in spellbook (Friend type)

TODO

-add Ally graphics
-Implement Ally.damage special ally stat stuff
-implement charge gauge mechanics
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/gameflow.xlsx
+++ b/Typocrypha/Assets/excel/gameflow.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="55">
   <si>
     <t>INTRO</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>END_DIALOGUE</t>
+  </si>
+  <si>
+    <t>Illyia</t>
+  </si>
+  <si>
+    <t>ALLY</t>
+  </si>
+  <si>
+    <t>Dahlia</t>
   </si>
 </sst>
 </file>
@@ -531,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,18 +702,18 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -712,280 +721,250 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15">
-        <v>0.5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25">
-        <v>0.75</v>
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>0.75</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" t="s">
-        <v>47</v>
-      </c>
-      <c r="G27" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" t="s">
-        <v>47</v>
-      </c>
-      <c r="G32" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -996,10 +975,10 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -1013,11 +992,57 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented spell registering and spellbook scroll sfx, added volume control to AudioPlayer
FILES ADDED:

several sfx

FILES MODIFIED:

Audioplayer.cs
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/gameflow.xlsx
+++ b/Typocrypha/Assets/excel/gameflow.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JTI-PC\unity_projects\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>START_SCENE</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>[set-bg=bg_battle_2]_</t>
+  </si>
+  <si>
+    <t>REGISTER</t>
+  </si>
+  <si>
+    <t>sword</t>
+  </si>
+  <si>
+    <t>spear</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
 </sst>
 </file>
@@ -447,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,31 +529,37 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -549,15 +567,15 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -565,7 +583,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -573,52 +591,60 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented better battle interrupt system
-Can now define arbitrary battle interrupt conditions in 'BattleInterrupts.cs' as bool function handles.
-System works in a very similar manner to the TextEvents system.
-You still have to specify in the gameflow file which enemies must be alive for the battle interrupt to take place (you can leave it empty, if no one needs to be alive).
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/gameflow.xlsx
+++ b/Typocrypha/Assets/excel/gameflow.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hughe\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JTI-PC\unity_projects\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gameflow" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>START_SCENE</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Lilim</t>
   </si>
   <si>
-    <t>Battle!</t>
-  </si>
-  <si>
     <t>tanuki</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>_</t>
   </si>
   <si>
-    <t>[set-bg=bg_battle_2]_</t>
-  </si>
-  <si>
     <t>REGISTER</t>
   </si>
   <si>
@@ -108,12 +102,27 @@
   </si>
   <si>
     <t>bgm_battle_a1</t>
+  </si>
+  <si>
+    <t>[set-bg=bg_battle_2]Battle!</t>
+  </si>
+  <si>
+    <t>INTERRUPT</t>
+  </si>
+  <si>
+    <t>END_INTERRUPT</t>
+  </si>
+  <si>
+    <t>check-health,0,0.5</t>
+  </si>
+  <si>
+    <t>Ow! That hurts!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,28 +467,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -490,7 +499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -498,13 +507,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -513,138 +522,160 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
         <v>11</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>